<commit_message>
Deploying to gh-pages from @ aehrc/genclipr-fhir-ig@02cc4c19141e33d25740b38c8ef66775f1672aa9 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-Finding.xlsx
+++ b/StructureDefinition-Finding.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="410">
   <si>
     <t>Path</t>
   </si>
@@ -882,40 +882,37 @@
 If the use case requires BodySite to be handled as a separate resource (e.g. to identify and track separately) then use the standard extension[ bodySite](http://hl7.org/fhir/R4/extension-bodysite.html).</t>
   </si>
   <si>
+    <t>http://hl7.org/fhir/ValueSet/body-site</t>
+  </si>
+  <si>
+    <t>&lt; 123037004 |Body structure|</t>
+  </si>
+  <si>
+    <t>OBX-20</t>
+  </si>
+  <si>
+    <t>targetSiteCode</t>
+  </si>
+  <si>
+    <t>718497002 |Inherent location|</t>
+  </si>
+  <si>
+    <t>Observation.method</t>
+  </si>
+  <si>
+    <t>How it was done</t>
+  </si>
+  <si>
+    <t>Indicates the mechanism used to perform the observation.</t>
+  </si>
+  <si>
+    <t>Only used if not implicit in code for Observation.code.</t>
+  </si>
+  <si>
+    <t>In some cases, method can impact results and is thus used for determining whether results can be compared or determining significance of results.</t>
+  </si>
+  <si>
     <t>example</t>
-  </si>
-  <si>
-    <t>Codes describing anatomical locations. May include laterality.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/body-site</t>
-  </si>
-  <si>
-    <t>&lt; 123037004 |Body structure|</t>
-  </si>
-  <si>
-    <t>OBX-20</t>
-  </si>
-  <si>
-    <t>targetSiteCode</t>
-  </si>
-  <si>
-    <t>718497002 |Inherent location|</t>
-  </si>
-  <si>
-    <t>Observation.method</t>
-  </si>
-  <si>
-    <t>How it was done</t>
-  </si>
-  <si>
-    <t>Indicates the mechanism used to perform the observation.</t>
-  </si>
-  <si>
-    <t>Only used if not implicit in code for Observation.code.</t>
-  </si>
-  <si>
-    <t>In some cases, method can impact results and is thus used for determining whether results can be compared or determining significance of results.</t>
   </si>
   <si>
     <t>Methods for simple observations.</t>
@@ -4570,7 +4567,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" hidden="true">
+    <row r="27">
       <c r="A27" t="s" s="2">
         <v>272</v>
       </c>
@@ -4586,7 +4583,7 @@
         <v>55</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>45</v>
@@ -4630,13 +4627,11 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="X27" s="2"/>
+      <c r="Y27" t="s" s="2">
         <v>276</v>
-      </c>
-      <c r="X27" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="Y27" t="s" s="2">
-        <v>278</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4672,24 +4667,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="AL27" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="AM27" t="s" s="2">
         <v>279</v>
       </c>
-      <c r="AL27" t="s" s="2">
+      <c r="AN27" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO27" t="s" s="2">
         <v>280</v>
-      </c>
-      <c r="AM27" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="AN27" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO27" t="s" s="2">
-        <v>282</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4715,16 +4710,16 @@
         <v>153</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="L28" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="M28" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="L28" t="s" s="2">
+      <c r="N28" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>287</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
@@ -4749,14 +4744,14 @@
         <v>45</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="X28" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="Y28" t="s" s="2">
         <v>288</v>
       </c>
-      <c r="Y28" t="s" s="2">
-        <v>289</v>
-      </c>
       <c r="Z28" t="s" s="2">
         <v>45</v>
       </c>
@@ -4773,7 +4768,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4794,10 +4789,10 @@
         <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="AM28" t="s" s="2">
         <v>290</v>
-      </c>
-      <c r="AM28" t="s" s="2">
-        <v>291</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
@@ -4808,7 +4803,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4831,16 +4826,16 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="K29" t="s" s="2">
         <v>293</v>
       </c>
-      <c r="K29" t="s" s="2">
+      <c r="L29" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>295</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>296</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4890,7 +4885,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4908,24 +4903,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="AL29" t="s" s="2">
         <v>297</v>
       </c>
-      <c r="AL29" t="s" s="2">
+      <c r="AM29" t="s" s="2">
         <v>298</v>
       </c>
-      <c r="AM29" t="s" s="2">
+      <c r="AN29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO29" t="s" s="2">
         <v>299</v>
-      </c>
-      <c r="AN29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO29" t="s" s="2">
-        <v>300</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4948,16 +4943,16 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="K30" t="s" s="2">
         <v>302</v>
       </c>
-      <c r="K30" t="s" s="2">
+      <c r="L30" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>304</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>305</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -5007,7 +5002,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5025,24 +5020,24 @@
         <v>45</v>
       </c>
       <c r="AK30" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="AL30" t="s" s="2">
         <v>306</v>
       </c>
-      <c r="AL30" t="s" s="2">
+      <c r="AM30" t="s" s="2">
         <v>307</v>
       </c>
-      <c r="AM30" t="s" s="2">
+      <c r="AN30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO30" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="AN30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO30" t="s" s="2">
-        <v>309</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5065,19 +5060,19 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="K31" t="s" s="2">
         <v>311</v>
       </c>
-      <c r="K31" t="s" s="2">
+      <c r="L31" t="s" s="2">
         <v>312</v>
       </c>
-      <c r="L31" t="s" s="2">
+      <c r="M31" t="s" s="2">
         <v>313</v>
       </c>
-      <c r="M31" t="s" s="2">
+      <c r="N31" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>315</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>45</v>
@@ -5126,7 +5121,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5138,19 +5133,19 @@
         <v>45</v>
       </c>
       <c r="AI31" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK31" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL31" t="s" s="2">
         <v>316</v>
       </c>
-      <c r="AJ31" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK31" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL31" t="s" s="2">
+      <c r="AM31" t="s" s="2">
         <v>317</v>
-      </c>
-      <c r="AM31" t="s" s="2">
-        <v>318</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5161,7 +5156,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5187,10 +5182,10 @@
         <v>57</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>321</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5241,7 +5236,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5265,7 +5260,7 @@
         <v>45</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5276,7 +5271,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5305,7 +5300,7 @@
         <v>102</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>104</v>
@@ -5358,7 +5353,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5382,7 +5377,7 @@
         <v>45</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5393,11 +5388,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5419,10 +5414,10 @@
         <v>101</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="L34" t="s" s="2">
         <v>329</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>330</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>104</v>
@@ -5477,7 +5472,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5512,7 +5507,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5535,13 +5530,13 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="K35" t="s" s="2">
         <v>333</v>
       </c>
-      <c r="K35" t="s" s="2">
+      <c r="L35" t="s" s="2">
         <v>334</v>
-      </c>
-      <c r="L35" t="s" s="2">
-        <v>335</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5592,7 +5587,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5601,7 +5596,7 @@
         <v>55</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>67</v>
@@ -5613,10 +5608,10 @@
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="AM35" t="s" s="2">
         <v>337</v>
-      </c>
-      <c r="AM35" t="s" s="2">
-        <v>338</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5627,7 +5622,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5650,13 +5645,13 @@
         <v>45</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>340</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>341</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5707,7 +5702,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5716,7 +5711,7 @@
         <v>55</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>67</v>
@@ -5728,10 +5723,10 @@
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5742,7 +5737,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5768,16 +5763,16 @@
         <v>153</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>344</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="M37" t="s" s="2">
         <v>345</v>
       </c>
-      <c r="M37" t="s" s="2">
+      <c r="N37" t="s" s="2">
         <v>346</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>347</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5805,11 +5800,11 @@
         <v>79</v>
       </c>
       <c r="X37" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="Y37" t="s" s="2">
         <v>348</v>
       </c>
-      <c r="Y37" t="s" s="2">
-        <v>349</v>
-      </c>
       <c r="Z37" t="s" s="2">
         <v>45</v>
       </c>
@@ -5826,7 +5821,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5844,10 +5839,10 @@
         <v>45</v>
       </c>
       <c r="AK37" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="AL37" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="AL37" t="s" s="2">
-        <v>351</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>262</v>
@@ -5861,7 +5856,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5887,16 +5882,16 @@
         <v>153</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>353</v>
       </c>
-      <c r="L38" t="s" s="2">
+      <c r="M38" t="s" s="2">
         <v>354</v>
       </c>
-      <c r="M38" t="s" s="2">
+      <c r="N38" t="s" s="2">
         <v>355</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>356</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
@@ -5921,14 +5916,14 @@
         <v>45</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="X38" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="Y38" t="s" s="2">
         <v>357</v>
       </c>
-      <c r="Y38" t="s" s="2">
-        <v>358</v>
-      </c>
       <c r="Z38" t="s" s="2">
         <v>45</v>
       </c>
@@ -5945,7 +5940,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -5963,10 +5958,10 @@
         <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="AL38" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="AL38" t="s" s="2">
-        <v>351</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>262</v>
@@ -5980,7 +5975,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6003,17 +5998,17 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="K39" t="s" s="2">
         <v>360</v>
       </c>
-      <c r="K39" t="s" s="2">
+      <c r="L39" t="s" s="2">
         <v>361</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>362</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6062,7 +6057,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6086,7 +6081,7 @@
         <v>45</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6097,7 +6092,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6123,10 +6118,10 @@
         <v>57</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>366</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>367</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -6177,7 +6172,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6198,10 +6193,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6212,7 +6207,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6235,16 +6230,16 @@
         <v>56</v>
       </c>
       <c r="J41" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="K41" t="s" s="2">
         <v>370</v>
       </c>
-      <c r="K41" t="s" s="2">
+      <c r="L41" t="s" s="2">
         <v>371</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="M41" t="s" s="2">
         <v>372</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>373</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
@@ -6294,7 +6289,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6315,10 +6310,10 @@
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="AM41" t="s" s="2">
         <v>374</v>
-      </c>
-      <c r="AM41" t="s" s="2">
-        <v>375</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6329,7 +6324,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6352,16 +6347,16 @@
         <v>56</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="K42" t="s" s="2">
         <v>377</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="L42" t="s" s="2">
         <v>378</v>
       </c>
-      <c r="L42" t="s" s="2">
+      <c r="M42" t="s" s="2">
         <v>379</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>380</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6411,7 +6406,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6432,10 +6427,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6446,7 +6441,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6469,19 +6464,19 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>383</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>384</v>
       </c>
-      <c r="M43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>386</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>45</v>
@@ -6530,7 +6525,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6551,10 +6546,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="AM43" t="s" s="2">
         <v>387</v>
-      </c>
-      <c r="AM43" t="s" s="2">
-        <v>388</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6565,7 +6560,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6591,10 +6586,10 @@
         <v>57</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>321</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6645,7 +6640,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6669,7 +6664,7 @@
         <v>45</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6680,7 +6675,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6709,7 +6704,7 @@
         <v>102</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M45" t="s" s="2">
         <v>104</v>
@@ -6762,7 +6757,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -6786,7 +6781,7 @@
         <v>45</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6797,11 +6792,11 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -6823,10 +6818,10 @@
         <v>101</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>329</v>
-      </c>
-      <c r="L46" t="s" s="2">
-        <v>330</v>
       </c>
       <c r="M46" t="s" s="2">
         <v>104</v>
@@ -6881,7 +6876,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6916,7 +6911,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6942,13 +6937,13 @@
         <v>153</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>393</v>
       </c>
-      <c r="L47" t="s" s="2">
+      <c r="M47" t="s" s="2">
         <v>394</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>395</v>
       </c>
       <c r="N47" t="s" s="2">
         <v>167</v>
@@ -6976,14 +6971,14 @@
         <v>45</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="X47" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="Y47" t="s" s="2">
         <v>396</v>
       </c>
-      <c r="Y47" t="s" s="2">
-        <v>397</v>
-      </c>
       <c r="Z47" t="s" s="2">
         <v>45</v>
       </c>
@@ -7000,7 +6995,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>55</v>
@@ -7018,7 +7013,7 @@
         <v>45</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>171</v>
@@ -7035,7 +7030,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7061,13 +7056,13 @@
         <v>231</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="L48" t="s" s="2">
         <v>233</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="N48" t="s" s="2">
         <v>235</v>
@@ -7119,7 +7114,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7137,7 +7132,7 @@
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>239</v>
@@ -7154,7 +7149,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7180,13 +7175,13 @@
         <v>153</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>404</v>
       </c>
-      <c r="L49" t="s" s="2">
+      <c r="M49" t="s" s="2">
         <v>405</v>
-      </c>
-      <c r="M49" t="s" s="2">
-        <v>406</v>
       </c>
       <c r="N49" t="s" s="2">
         <v>246</v>
@@ -7238,7 +7233,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7273,7 +7268,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7357,7 +7352,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7392,7 +7387,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7418,16 +7413,16 @@
         <v>45</v>
       </c>
       <c r="K51" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>409</v>
       </c>
-      <c r="L51" t="s" s="2">
-        <v>410</v>
-      </c>
       <c r="M51" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="N51" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>315</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7476,7 +7471,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7497,10 +7492,10 @@
         <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="AM51" t="s" s="2">
         <v>317</v>
-      </c>
-      <c r="AM51" t="s" s="2">
-        <v>318</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>

</xml_diff>